<commit_message>
Updated for comparing Expected and Actual response
</commit_message>
<xml_diff>
--- a/test_data/actor_test_data.xlsx
+++ b/test_data/actor_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\driver\PythonProject\PythonProject\api-framework\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43407E1-0164-4526-BA4B-D54739640391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FA5952-A8A0-4A9F-B582-E8F9362724B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,61 +84,61 @@
   <si>
     <t xml:space="preserve">  {
     "first_name": "Dilip",
-    "last_name": "Kumar",  
+    "last_name": "Kumar"
 }</t>
   </si>
   <si>
     <t xml:space="preserve">  {
     "first_name": "Amir",
-    "last_name": "Khan",  
+    "last_name": "Khan"
 }</t>
   </si>
   <si>
     <t xml:space="preserve">  {
     "first_name": "Shahrukh",
-    "last_name": "Khan",  
+    "last_name": "Khan"
 }</t>
   </si>
   <si>
     <t xml:space="preserve">  {
     "first_name": "Salman",
-    "last_name": "Khan",  
+    "last_name": "Khan"
 }</t>
   </si>
   <si>
     <t xml:space="preserve">  {
     "first_name": "Amitabh",
-    "last_name": "Bachchan",  
+    "last_name": "Bachchan"
 }</t>
   </si>
   <si>
     <t xml:space="preserve">  {
     "first_name": "Akshay",
-    "last_name": "Kumar",  
+    "last_name": "Kumar"
 }</t>
   </si>
   <si>
     <t xml:space="preserve">  {
     "first_name": "Varun",
-    "last_name": "Dhawan",  
+    "last_name": "Dhawan"
 }</t>
   </si>
   <si>
     <t xml:space="preserve">  {
     "first_name": "Ranbir",
-    "last_name": "Kapoor",  
+    "last_name": "Kapoor"
 }</t>
   </si>
   <si>
     <t xml:space="preserve">  {
     "first_name": "Ranvir",
-    "last_name": "Singh",  
+    "last_name": "Singh"
 }</t>
   </si>
   <si>
     <t xml:space="preserve">  {
     "first_name": "Rishi",
-    "last_name": "Kapoor",  
+    "last_name": "Kapoor"
 }</t>
   </si>
 </sst>
@@ -187,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -195,6 +195,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,15 +500,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" activeCellId="1" sqref="E23 G7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C7" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="3" max="3" width="30" style="3" customWidth="1"/>
     <col min="4" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
@@ -546,7 +547,7 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -557,7 +558,7 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -568,7 +569,7 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -579,7 +580,7 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -590,7 +591,7 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -601,7 +602,7 @@
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -612,7 +613,7 @@
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -623,7 +624,7 @@
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -634,7 +635,7 @@
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -645,7 +646,7 @@
       <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Upadated for value compare
Updated for value compare previously it was only comparing key from the actual response now comparing key and value both from responses
</commit_message>
<xml_diff>
--- a/test_data/actor_test_data.xlsx
+++ b/test_data/actor_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\driver\PythonProject\PythonProject\api-framework\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FA5952-A8A0-4A9F-B582-E8F9362724B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719B3113-D539-4F3C-866A-31F8872B0228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>first_name</t>
   </si>
@@ -31,12 +31,6 @@
     <t>Dilip</t>
   </si>
   <si>
-    <t xml:space="preserve"> Kumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amir </t>
-  </si>
-  <si>
     <t>Khan</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
   </si>
   <si>
     <t>Singh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rishi </t>
   </si>
   <si>
     <t>expected_response</t>
@@ -140,6 +131,12 @@
     "first_name": "Rishi",
     "last_name": "Kapoor"
 }</t>
+  </si>
+  <si>
+    <t>Amir</t>
+  </si>
+  <si>
+    <t>Rishi</t>
   </si>
 </sst>
 </file>
@@ -195,7 +192,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,15 +499,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C7" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="30" style="3" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
     <col min="4" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
@@ -527,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -540,114 +539,114 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>22</v>
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>